<commit_message>
update end of 2019
</commit_message>
<xml_diff>
--- a/data/countries.xlsx
+++ b/data/countries.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\rufibach\01_personal\30_mobilitaet\travel\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\rufibach\01_personal\05_Sport\40_reporting\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -407,8 +407,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T12" sqref="T12"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="K48" sqref="K48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1055,6 +1055,9 @@
       <c r="E47" s="3">
         <v>5</v>
       </c>
+      <c r="K47" s="1">
+        <v>105.25</v>
+      </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
@@ -1079,6 +1082,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <FileSizeOrChildItemCount xmlns="d92fc194-eb53-4f7a-b45f-993e54cb3c65">17 KB</FileSizeOrChildItemCount>
@@ -1091,15 +1103,6 @@
     <_dlc_ExpireDateSaved xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1294,6 +1297,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77A77888-53C6-464C-8A2C-8B68487BDD80}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0ECEC803-CE3A-41AA-8A6B-E3884C13B2B5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
@@ -1308,14 +1319,6 @@
     <ds:schemaRef ds:uri="1071F304-F5D9-4CC4-AFCF-D37DA46A96D4"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77A77888-53C6-464C-8A2C-8B68487BDD80}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>